<commit_message>
add name to scatter matrix
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Projects\Python\first-coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4070E0-41B5-4829-8C00-3B4748465AD6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6D643A-22F1-4D83-BAA2-9B93F3D343CF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1627,20 +1627,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G411"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +1708,7 @@
         <v>0.3039581777445855</v>
       </c>
       <c r="G3">
-        <v>0.30151007882727138</v>
+        <v>0.30151007882727121</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1729,7 +1731,7 @@
         <v>0.36567834681042227</v>
       </c>
       <c r="G4">
-        <v>0.56588040634819403</v>
+        <v>0.56588040634819392</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1752,7 +1754,7 @@
         <v>0.26900198281559817</v>
       </c>
       <c r="G5">
-        <v>3.6318954480904407E-2</v>
+        <v>3.6318954480904463E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1775,7 +1777,7 @@
         <v>0.31747269890795632</v>
       </c>
       <c r="G6">
-        <v>0.32741493016314321</v>
+        <v>0.32741493016314288</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1821,7 +1823,7 @@
         <v>0.32199367088607589</v>
       </c>
       <c r="G8">
-        <v>0.21631878365015289</v>
+        <v>0.21631878365015281</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1844,7 +1846,7 @@
         <v>0.29133858267716528</v>
       </c>
       <c r="G9">
-        <v>8.9587994269960641E-2</v>
+        <v>8.9587994269960655E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1867,7 +1869,7 @@
         <v>0.29578488372093031</v>
       </c>
       <c r="G10">
-        <v>8.3483891017802889E-2</v>
+        <v>8.3483891017802916E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1890,7 +1892,7 @@
         <v>0.32664526484751211</v>
       </c>
       <c r="G11">
-        <v>0.20255409976961161</v>
+        <v>0.20255409976961181</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1936,7 +1938,7 @@
         <v>0.26549249836921068</v>
       </c>
       <c r="G13">
-        <v>6.2487670645710668E-2</v>
+        <v>6.2487670645710758E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1959,7 +1961,7 @@
         <v>0.28926794598436389</v>
       </c>
       <c r="G14">
-        <v>0.10465835583335791</v>
+        <v>0.104658355833358</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1982,7 +1984,7 @@
         <v>0.27705922396187882</v>
       </c>
       <c r="G15">
-        <v>9.8119033050964463E-2</v>
+        <v>9.8119033050964435E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2005,7 +2007,7 @@
         <v>0.31697819314641751</v>
       </c>
       <c r="G16">
-        <v>0.41246248501492011</v>
+        <v>0.41246248501492022</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2028,7 +2030,7 @@
         <v>0.30350484712900822</v>
       </c>
       <c r="G17">
-        <v>0.1583683215052718</v>
+        <v>0.15836832150527189</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2051,7 +2053,7 @@
         <v>0.33143322475570031</v>
       </c>
       <c r="G18">
-        <v>0.32508289322590811</v>
+        <v>0.32508289322590778</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2074,7 +2076,7 @@
         <v>0.32430278884462149</v>
       </c>
       <c r="G19">
-        <v>0.41466128279328601</v>
+        <v>0.41466128279328612</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2097,7 +2099,7 @@
         <v>0.29773226042428669</v>
       </c>
       <c r="G20">
-        <v>0.35599266685569569</v>
+        <v>0.35599266685569542</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2120,7 +2122,7 @@
         <v>0.31697819314641751</v>
       </c>
       <c r="G21">
-        <v>0.27243801383263011</v>
+        <v>0.27243801383263022</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2166,7 +2168,7 @@
         <v>0.27724795640326982</v>
       </c>
       <c r="G23">
-        <v>8.8215450895405986E-2</v>
+        <v>8.8215450895405972E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2189,7 +2191,7 @@
         <v>0.26549249836921068</v>
       </c>
       <c r="G24">
-        <v>4.1750148966693969E-2</v>
+        <v>4.1750148966694003E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2212,7 +2214,7 @@
         <v>0.28283530229325921</v>
       </c>
       <c r="G25">
-        <v>0.23087311775675201</v>
+        <v>0.2308731177567519</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2235,7 +2237,7 @@
         <v>0.30833333333333329</v>
       </c>
       <c r="G26">
-        <v>0.26178260688625948</v>
+        <v>0.26178260688625937</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2258,7 +2260,7 @@
         <v>0.35207612456747411</v>
       </c>
       <c r="G27">
-        <v>0.55349429749151069</v>
+        <v>0.55349429749151124</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2281,7 +2283,7 @@
         <v>0.33775933609958508</v>
       </c>
       <c r="G28">
-        <v>0.32245514304589218</v>
+        <v>0.32245514304589179</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2304,7 +2306,7 @@
         <v>0.28263888888888888</v>
       </c>
       <c r="G29">
-        <v>0.2416721731204946</v>
+        <v>0.24167217312049469</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2327,7 +2329,7 @@
         <v>0.33692052980132448</v>
       </c>
       <c r="G30">
-        <v>0.4309301533722979</v>
+        <v>0.43093015337229801</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2373,7 +2375,7 @@
         <v>0.31452859350850082</v>
       </c>
       <c r="G32">
-        <v>0.41663760201859762</v>
+        <v>0.41663760201859729</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2396,7 +2398,7 @@
         <v>0.32533972821742613</v>
       </c>
       <c r="G33">
-        <v>0.38104796164173288</v>
+        <v>0.38104796164173271</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2442,7 +2444,7 @@
         <v>0.3256</v>
       </c>
       <c r="G35">
-        <v>0.44616227270586839</v>
+        <v>0.44616227270586828</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2465,7 +2467,7 @@
         <v>0.32224861441013458</v>
       </c>
       <c r="G36">
-        <v>0.32583098568010382</v>
+        <v>0.32583098568010371</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2488,7 +2490,7 @@
         <v>0.29904481998530491</v>
       </c>
       <c r="G37">
-        <v>0.27847634909021041</v>
+        <v>0.27847634909021018</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2511,7 +2513,7 @@
         <v>0.28303198887343528</v>
       </c>
       <c r="G38">
-        <v>0.24954317232878881</v>
+        <v>0.249543172328789</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2534,7 +2536,7 @@
         <v>0.29992630803242448</v>
       </c>
       <c r="G39">
-        <v>0.32299152696344269</v>
+        <v>0.32299152696344258</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2557,7 +2559,7 @@
         <v>0.3192156862745098</v>
       </c>
       <c r="G40">
-        <v>0.45635844229657269</v>
+        <v>0.45635844229657241</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2580,7 +2582,7 @@
         <v>0.27370544720914591</v>
       </c>
       <c r="G41">
-        <v>6.0440373591603203E-2</v>
+        <v>6.0440373591603223E-2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2649,7 +2651,7 @@
         <v>0.35608048993875768</v>
       </c>
       <c r="G44">
-        <v>0.47438508046271372</v>
+        <v>0.47438508046271338</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2672,7 +2674,7 @@
         <v>0.30509745127436277</v>
       </c>
       <c r="G45">
-        <v>0.16792041547170669</v>
+        <v>0.1679204154717068</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2695,7 +2697,7 @@
         <v>0.29729729729729731</v>
       </c>
       <c r="G46">
-        <v>0.167565790821322</v>
+        <v>0.16756579082132211</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2718,7 +2720,7 @@
         <v>0.29450072358900142</v>
       </c>
       <c r="G47">
-        <v>0.15040828309125909</v>
+        <v>0.1504082830912592</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2741,7 +2743,7 @@
         <v>0.30578512396694207</v>
       </c>
       <c r="G48">
-        <v>0.31114805007681873</v>
+        <v>0.31114805007681851</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2764,7 +2766,7 @@
         <v>0.33062550771730298</v>
       </c>
       <c r="G49">
-        <v>0.32806314968799488</v>
+        <v>0.32806314968799483</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2787,7 +2789,7 @@
         <v>0.29009265858873839</v>
       </c>
       <c r="G50">
-        <v>0.1821300648185018</v>
+        <v>0.18213006481850169</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2810,7 +2812,7 @@
         <v>0.33470394736842107</v>
       </c>
       <c r="G51">
-        <v>0.26950704378774681</v>
+        <v>0.26950704378774648</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2833,7 +2835,7 @@
         <v>0.28621659634317859</v>
       </c>
       <c r="G52">
-        <v>0.30258381248704308</v>
+        <v>0.30258381248704258</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2856,7 +2858,7 @@
         <v>0.28702397743300417</v>
       </c>
       <c r="G53">
-        <v>0.22711854030396059</v>
+        <v>0.22711854030396039</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2879,7 +2881,7 @@
         <v>0.29664723032069967</v>
       </c>
       <c r="G54">
-        <v>0.23172854603416351</v>
+        <v>0.2317285460341634</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2948,7 +2950,7 @@
         <v>0.30950570342205319</v>
       </c>
       <c r="G57">
-        <v>0.2096504445581048</v>
+        <v>0.20965044455810461</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2994,7 +2996,7 @@
         <v>0.2988252569750367</v>
       </c>
       <c r="G59">
-        <v>0.30042659671998811</v>
+        <v>0.300426596719988</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3040,7 +3042,7 @@
         <v>0.29050678087080661</v>
       </c>
       <c r="G61">
-        <v>0.23443730449930619</v>
+        <v>0.23443730449930611</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3063,7 +3065,7 @@
         <v>0.29904481998530491</v>
       </c>
       <c r="G62">
-        <v>0.3275353367625547</v>
+        <v>0.32753533676255481</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3086,7 +3088,7 @@
         <v>0.28621659634317859</v>
       </c>
       <c r="G63">
-        <v>0.23573777993873771</v>
+        <v>0.2357377799387374</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3109,7 +3111,7 @@
         <v>0.2489296636085627</v>
       </c>
       <c r="G64">
-        <v>5.6474815785505908E-2</v>
+        <v>5.647481578550588E-2</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3132,7 +3134,7 @@
         <v>0.2492345376607471</v>
       </c>
       <c r="G65">
-        <v>5.6699128291298022E-2</v>
+        <v>5.6699128291297987E-2</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3155,7 +3157,7 @@
         <v>0.29471397538015931</v>
       </c>
       <c r="G66">
-        <v>0.130959370639471</v>
+        <v>0.13095937063947091</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3178,7 +3180,7 @@
         <v>0.2489296636085627</v>
       </c>
       <c r="G67">
-        <v>5.6474815785505943E-2</v>
+        <v>5.6474815785505873E-2</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3201,7 +3203,7 @@
         <v>0.26308985132514551</v>
       </c>
       <c r="G68">
-        <v>6.8194492152257161E-2</v>
+        <v>6.8194492152257064E-2</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3224,7 +3226,7 @@
         <v>0.30950570342205319</v>
       </c>
       <c r="G69">
-        <v>0.18261169014219941</v>
+        <v>0.1826116901421995</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3247,7 +3249,7 @@
         <v>0.26308985132514551</v>
       </c>
       <c r="G70">
-        <v>6.8194492152257105E-2</v>
+        <v>6.8194492152257091E-2</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3270,7 +3272,7 @@
         <v>0.29365079365079372</v>
       </c>
       <c r="G71">
-        <v>0.15307312831158951</v>
+        <v>0.1530731283115894</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3293,7 +3295,7 @@
         <v>0.2964311726147123</v>
       </c>
       <c r="G72">
-        <v>0.12597826790810701</v>
+        <v>0.12597826790810709</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3316,7 +3318,7 @@
         <v>0.30192878338278928</v>
       </c>
       <c r="G73">
-        <v>0.2194651461776998</v>
+        <v>0.21946514617769991</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3339,7 +3341,7 @@
         <v>0.3138010794140324</v>
       </c>
       <c r="G74">
-        <v>0.20065746015574951</v>
+        <v>0.20065746015574959</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3408,7 +3410,7 @@
         <v>0.27518593644354289</v>
       </c>
       <c r="G77">
-        <v>6.9040264581189642E-2</v>
+        <v>6.9040264581189698E-2</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3431,7 +3433,7 @@
         <v>0.29751461988304101</v>
       </c>
       <c r="G78">
-        <v>0.13300182931396651</v>
+        <v>0.1330018293139664</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3454,7 +3456,7 @@
         <v>0.34144295302013422</v>
       </c>
       <c r="G79">
-        <v>0.128441481828339</v>
+        <v>0.12844148182833889</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3477,7 +3479,7 @@
         <v>0.30647590361445781</v>
       </c>
       <c r="G80">
-        <v>7.9915085392038593E-2</v>
+        <v>7.9915085392038607E-2</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3500,7 +3502,7 @@
         <v>0.22338090010976949</v>
       </c>
       <c r="G81">
-        <v>3.1539141527111591E-3</v>
+        <v>3.153914152711163E-3</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3523,7 +3525,7 @@
         <v>0.36145648312611012</v>
       </c>
       <c r="G82">
-        <v>0.22157709889984159</v>
+        <v>0.2215770988998414</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3546,7 +3548,7 @@
         <v>0.28283530229325921</v>
       </c>
       <c r="G83">
-        <v>3.9887089535328227E-2</v>
+        <v>3.9887089535328248E-2</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3592,7 +3594,7 @@
         <v>0.30532633158289568</v>
       </c>
       <c r="G85">
-        <v>8.6654395018378252E-2</v>
+        <v>8.665439501837828E-2</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3615,7 +3617,7 @@
         <v>0.31599378881987578</v>
       </c>
       <c r="G86">
-        <v>8.8716536170713511E-2</v>
+        <v>8.8716536170713456E-2</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3661,7 +3663,7 @@
         <v>0.30373134328358209</v>
       </c>
       <c r="G88">
-        <v>8.7783923060744923E-2</v>
+        <v>8.7783923060744867E-2</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3684,7 +3686,7 @@
         <v>0.28988603988603989</v>
       </c>
       <c r="G89">
-        <v>3.3958404962228822E-2</v>
+        <v>3.3958404962228857E-2</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3707,7 +3709,7 @@
         <v>0.26497395833333331</v>
       </c>
       <c r="G90">
-        <v>1.2945777674551609E-2</v>
+        <v>1.2945777674551641E-2</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3730,7 +3732,7 @@
         <v>0.26497395833333331</v>
       </c>
       <c r="G91">
-        <v>1.2945777674551609E-2</v>
+        <v>1.2945777674551641E-2</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3753,7 +3755,7 @@
         <v>0.2988252569750367</v>
       </c>
       <c r="G92">
-        <v>7.5844026240084877E-2</v>
+        <v>7.5844026240084933E-2</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3776,7 +3778,7 @@
         <v>0.29009265858873839</v>
       </c>
       <c r="G93">
-        <v>4.1630467434556423E-2</v>
+        <v>4.163046743455643E-2</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3799,7 +3801,7 @@
         <v>0.28803963198867649</v>
       </c>
       <c r="G94">
-        <v>3.3219691515419633E-2</v>
+        <v>3.3219691515419619E-2</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3822,7 +3824,7 @@
         <v>0.33470394736842107</v>
       </c>
       <c r="G95">
-        <v>0.1224741833463676</v>
+        <v>0.12247418334636739</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3845,7 +3847,7 @@
         <v>0.26989389920424411</v>
       </c>
       <c r="G96">
-        <v>1.558841210819761E-2</v>
+        <v>1.558841210819762E-2</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3868,7 +3870,7 @@
         <v>0.26497395833333331</v>
       </c>
       <c r="G97">
-        <v>1.2945777674551609E-2</v>
+        <v>1.294577767455163E-2</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3891,7 +3893,7 @@
         <v>0.29029957203994289</v>
       </c>
       <c r="G98">
-        <v>3.9515485326188572E-2</v>
+        <v>3.95154853261886E-2</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3914,7 +3916,7 @@
         <v>0.28030303030303028</v>
       </c>
       <c r="G99">
-        <v>2.562167467035429E-2</v>
+        <v>2.5621674670354321E-2</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3937,7 +3939,7 @@
         <v>0.29259525521207758</v>
       </c>
       <c r="G100">
-        <v>4.2176921946150719E-2</v>
+        <v>4.2176921946150733E-2</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3960,7 +3962,7 @@
         <v>0.32199367088607589</v>
       </c>
       <c r="G101">
-        <v>9.0185110656104586E-2</v>
+        <v>9.0185110656104475E-2</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3983,7 +3985,7 @@
         <v>0.29009265858873839</v>
       </c>
       <c r="G102">
-        <v>4.1630467434556402E-2</v>
+        <v>4.1630467434556437E-2</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4006,7 +4008,7 @@
         <v>0.31428571428571428</v>
       </c>
       <c r="G103">
-        <v>8.383031151752364E-2</v>
+        <v>8.3830311517523695E-2</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4052,7 +4054,7 @@
         <v>0.29009265858873839</v>
       </c>
       <c r="G105">
-        <v>4.1630467434556423E-2</v>
+        <v>4.1630467434556402E-2</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4075,7 +4077,7 @@
         <v>0.29009265858873839</v>
       </c>
       <c r="G106">
-        <v>4.1630467434556423E-2</v>
+        <v>4.1630467434556402E-2</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4098,7 +4100,7 @@
         <v>0.26497395833333331</v>
       </c>
       <c r="G107">
-        <v>1.2945777674551609E-2</v>
+        <v>1.294577767455163E-2</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4167,7 +4169,7 @@
         <v>0.30464071856287422</v>
       </c>
       <c r="G110">
-        <v>5.4232318803096757E-2</v>
+        <v>5.4232318803096841E-2</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4190,7 +4192,7 @@
         <v>0.28844790928419561</v>
       </c>
       <c r="G111">
-        <v>5.0243771559276278E-2</v>
+        <v>5.0243771559276298E-2</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4213,7 +4215,7 @@
         <v>0.27593220338983049</v>
       </c>
       <c r="G112">
-        <v>3.2075545506133167E-2</v>
+        <v>3.207554550613323E-2</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4236,7 +4238,7 @@
         <v>0.26514657980456019</v>
       </c>
       <c r="G113">
-        <v>2.101262728767718E-2</v>
+        <v>2.1012627287677211E-2</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4259,7 +4261,7 @@
         <v>0.28107734806629842</v>
       </c>
       <c r="G114">
-        <v>3.3688524283479827E-2</v>
+        <v>3.3688524283479883E-2</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4282,7 +4284,7 @@
         <v>0.32982171799027549</v>
       </c>
       <c r="G115">
-        <v>0.25149729903050261</v>
+        <v>0.25149729903050227</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4351,7 +4353,7 @@
         <v>0.26514657980456019</v>
       </c>
       <c r="G118">
-        <v>2.101262728767718E-2</v>
+        <v>2.1012627287677211E-2</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4374,7 +4376,7 @@
         <v>0.26514657980456019</v>
       </c>
       <c r="G119">
-        <v>2.101262728767719E-2</v>
+        <v>2.1012627287677211E-2</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -4397,7 +4399,7 @@
         <v>0.28501400560224088</v>
       </c>
       <c r="G120">
-        <v>4.1286541128545157E-2</v>
+        <v>4.1286541128545233E-2</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4443,7 +4445,7 @@
         <v>0.26514657980456019</v>
       </c>
       <c r="G122">
-        <v>2.101262728767719E-2</v>
+        <v>2.1012627287677211E-2</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4466,7 +4468,7 @@
         <v>0.26514657980456019</v>
       </c>
       <c r="G123">
-        <v>2.101262728767719E-2</v>
+        <v>2.1012627287677201E-2</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4489,7 +4491,7 @@
         <v>0.26514657980456019</v>
       </c>
       <c r="G124">
-        <v>2.101262728767719E-2</v>
+        <v>2.1012627287677201E-2</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4512,7 +4514,7 @@
         <v>0.26258064516129032</v>
       </c>
       <c r="G125">
-        <v>2.6723795031407319E-2</v>
+        <v>2.672379503140733E-2</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4673,7 +4675,7 @@
         <v>0.33916666666666673</v>
       </c>
       <c r="G132">
-        <v>0.1674460026455325</v>
+        <v>0.1674460026455323</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4696,7 +4698,7 @@
         <v>0.35954063604240277</v>
       </c>
       <c r="G133">
-        <v>0.22437042238672469</v>
+        <v>0.22437042238672461</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4742,7 +4744,7 @@
         <v>0.29238505747126442</v>
       </c>
       <c r="G135">
-        <v>5.1144371288927563E-2</v>
+        <v>5.1144371288927577E-2</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4765,7 +4767,7 @@
         <v>0.33197389885807499</v>
       </c>
       <c r="G136">
-        <v>0.1449696342955849</v>
+        <v>0.1449696342955851</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4788,7 +4790,7 @@
         <v>0.30464071856287422</v>
       </c>
       <c r="G137">
-        <v>8.5650108900689734E-2</v>
+        <v>8.5650108900689678E-2</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4811,7 +4813,7 @@
         <v>0.31821735731039869</v>
       </c>
       <c r="G138">
-        <v>0.1229197703848621</v>
+        <v>0.1229197703848619</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4857,7 +4859,7 @@
         <v>0.27762619372442021</v>
       </c>
       <c r="G140">
-        <v>3.1327324193650759E-2</v>
+        <v>3.1327324193650752E-2</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -4880,7 +4882,7 @@
         <v>0.3080999242997729</v>
       </c>
       <c r="G141">
-        <v>0.14652667513898421</v>
+        <v>0.1465266751389841</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -4903,7 +4905,7 @@
         <v>0.2919655667144907</v>
       </c>
       <c r="G142">
-        <v>5.8740813339906141E-2</v>
+        <v>5.8740813339906169E-2</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -4949,7 +4951,7 @@
         <v>0.29729729729729731</v>
       </c>
       <c r="G144">
-        <v>6.9303303021427745E-2</v>
+        <v>6.9303303021427731E-2</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -4972,7 +4974,7 @@
         <v>0.26882430647291938</v>
       </c>
       <c r="G145">
-        <v>2.656970765163693E-2</v>
+        <v>2.6569707651636951E-2</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4995,7 +4997,7 @@
         <v>0.36371760500446831</v>
       </c>
       <c r="G146">
-        <v>0.37072366695562442</v>
+        <v>0.37072366695562392</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -5018,7 +5020,7 @@
         <v>0.31331793687451892</v>
       </c>
       <c r="G147">
-        <v>0.16201724420401631</v>
+        <v>0.1620172442040162</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -5041,7 +5043,7 @@
         <v>0.27687074829931968</v>
       </c>
       <c r="G148">
-        <v>3.965494349821528E-2</v>
+        <v>3.9654943498215238E-2</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -5064,7 +5066,7 @@
         <v>0.34608843537414968</v>
       </c>
       <c r="G149">
-        <v>0.240108225466727</v>
+        <v>0.24010822546672711</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -5087,7 +5089,7 @@
         <v>0.35422106179286328</v>
       </c>
       <c r="G150">
-        <v>0.17186058020239661</v>
+        <v>0.1718605802023967</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -5110,7 +5112,7 @@
         <v>0.29578488372093031</v>
       </c>
       <c r="G151">
-        <v>6.3615082073269519E-2</v>
+        <v>6.3615082073269477E-2</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -5133,7 +5135,7 @@
         <v>0.28166089965397922</v>
       </c>
       <c r="G152">
-        <v>4.6843621492504928E-2</v>
+        <v>4.6843621492504907E-2</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -5156,7 +5158,7 @@
         <v>0.3403010033444816</v>
       </c>
       <c r="G153">
-        <v>0.18401735544960451</v>
+        <v>0.1840173554496044</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -5202,7 +5204,7 @@
         <v>0.29773226042428669</v>
       </c>
       <c r="G155">
-        <v>6.2575854660117322E-2</v>
+        <v>6.2575854660117308E-2</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -5225,7 +5227,7 @@
         <v>0.29557007988380529</v>
       </c>
       <c r="G156">
-        <v>3.8058379639074047E-2</v>
+        <v>3.8058379639074068E-2</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -5248,7 +5250,7 @@
         <v>0.34995700773860711</v>
       </c>
       <c r="G157">
-        <v>0.1826548791015562</v>
+        <v>0.18265487910155601</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5271,7 +5273,7 @@
         <v>0.3256</v>
       </c>
       <c r="G158">
-        <v>0.1264212347477964</v>
+        <v>0.12642123474779629</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5317,7 +5319,7 @@
         <v>0.29751461988304101</v>
       </c>
       <c r="G160">
-        <v>8.4021619635972197E-2</v>
+        <v>8.4021619635972239E-2</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5340,7 +5342,7 @@
         <v>0.3290218270008084</v>
       </c>
       <c r="G161">
-        <v>0.13264781777296511</v>
+        <v>0.13264781777296489</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5363,7 +5365,7 @@
         <v>0.3237867939538584</v>
       </c>
       <c r="G162">
-        <v>0.1072091906999612</v>
+        <v>0.1072091906999611</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5386,7 +5388,7 @@
         <v>0.32022029897718329</v>
       </c>
       <c r="G163">
-        <v>0.1129203584436914</v>
+        <v>0.1129203584436913</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5409,7 +5411,7 @@
         <v>0.30418535127055307</v>
       </c>
       <c r="G164">
-        <v>8.3535126792321945E-2</v>
+        <v>8.3535126792321876E-2</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -5432,7 +5434,7 @@
         <v>0.24847374847374851</v>
       </c>
       <c r="G165">
-        <v>1.8908931304774119E-2</v>
+        <v>1.890893130477413E-2</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5501,7 +5503,7 @@
         <v>0.2799174690508941</v>
       </c>
       <c r="G168">
-        <v>4.5632726336181477E-2</v>
+        <v>4.563272633618147E-2</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -5547,7 +5549,7 @@
         <v>0.24847374847374851</v>
       </c>
       <c r="G170">
-        <v>1.8908931304774119E-2</v>
+        <v>1.890893130477413E-2</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -5570,7 +5572,7 @@
         <v>0.24847374847374851</v>
       </c>
       <c r="G171">
-        <v>1.8908931304774119E-2</v>
+        <v>1.8908931304774109E-2</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -5593,7 +5595,7 @@
         <v>0.28661971830985922</v>
       </c>
       <c r="G172">
-        <v>4.5478638956411077E-2</v>
+        <v>4.5478638956411063E-2</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -5639,7 +5641,7 @@
         <v>0.30327868852459022</v>
       </c>
       <c r="G174">
-        <v>6.6491266244088285E-2</v>
+        <v>6.6491266244088201E-2</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -5662,7 +5664,7 @@
         <v>0.31428571428571428</v>
       </c>
       <c r="G175">
-        <v>0.13706653535268351</v>
+        <v>0.1370665353526834</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -5708,7 +5710,7 @@
         <v>0.26258064516129032</v>
       </c>
       <c r="G177">
-        <v>2.6723795031407309E-2</v>
+        <v>2.6723795031407319E-2</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5731,7 +5733,7 @@
         <v>0.29664723032069967</v>
       </c>
       <c r="G178">
-        <v>8.3689214172092227E-2</v>
+        <v>8.3689214172092172E-2</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5754,7 +5756,7 @@
         <v>0.29664723032069967</v>
       </c>
       <c r="G179">
-        <v>8.3689214172092186E-2</v>
+        <v>8.3689214172092199E-2</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -5777,7 +5779,7 @@
         <v>0.36274509803921567</v>
       </c>
       <c r="G180">
-        <v>0.2233722108818024</v>
+        <v>0.22337221088180251</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -5800,7 +5802,7 @@
         <v>0.29664723032069967</v>
       </c>
       <c r="G181">
-        <v>8.3689214172092255E-2</v>
+        <v>8.3689214172092227E-2</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -5823,7 +5825,7 @@
         <v>0.26258064516129032</v>
       </c>
       <c r="G182">
-        <v>2.6723795031407309E-2</v>
+        <v>2.672379503140733E-2</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -5846,7 +5848,7 @@
         <v>0.26258064516129032</v>
       </c>
       <c r="G183">
-        <v>2.6723795031407319E-2</v>
+        <v>2.672379503140734E-2</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -5955,7 +5957,7 @@
         <v>0.2663612565445026</v>
       </c>
       <c r="G188">
-        <v>2.245968152892279E-2</v>
+        <v>2.24596815289228E-2</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -6001,7 +6003,7 @@
         <v>0.2663612565445026</v>
       </c>
       <c r="G190">
-        <v>2.24596815289228E-2</v>
+        <v>2.2459681528922779E-2</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -6024,7 +6026,7 @@
         <v>0.29009265858873839</v>
       </c>
       <c r="G191">
-        <v>5.9417325868401559E-2</v>
+        <v>5.9417325868401608E-2</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -6047,7 +6049,7 @@
         <v>0.31452859350850082</v>
       </c>
       <c r="G192">
-        <v>0.1223155744339349</v>
+        <v>0.1223155744339347</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -6070,7 +6072,7 @@
         <v>0.30532633158289568</v>
       </c>
       <c r="G193">
-        <v>7.483023848800173E-2</v>
+        <v>7.4830238488001799E-2</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -6093,7 +6095,7 @@
         <v>0.31452859350850082</v>
       </c>
       <c r="G194">
-        <v>0.1223155744339349</v>
+        <v>0.1223155744339347</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -6116,7 +6118,7 @@
         <v>0.31477184841453981</v>
       </c>
       <c r="G195">
-        <v>0.10155876123392189</v>
+        <v>0.101558761233922</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -6139,7 +6141,7 @@
         <v>0.2663612565445026</v>
       </c>
       <c r="G196">
-        <v>2.245968152892279E-2</v>
+        <v>2.2459681528922811E-2</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -6185,7 +6187,7 @@
         <v>0.29838709677419362</v>
       </c>
       <c r="G198">
-        <v>6.5355675224869209E-2</v>
+        <v>6.5355675224869195E-2</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -6231,7 +6233,7 @@
         <v>0.28601546029515112</v>
       </c>
       <c r="G200">
-        <v>5.8263301572259923E-2</v>
+        <v>5.8263301572259868E-2</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -6254,7 +6256,7 @@
         <v>0.32638331996792302</v>
       </c>
       <c r="G201">
-        <v>0.15807015957211279</v>
+        <v>0.1580701595721129</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -6277,7 +6279,7 @@
         <v>0.34058577405857737</v>
       </c>
       <c r="G202">
-        <v>0.1912022765983252</v>
+        <v>0.19120227659832509</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -6300,7 +6302,7 @@
         <v>0.29238505747126442</v>
       </c>
       <c r="G203">
-        <v>6.1749717500524333E-2</v>
+        <v>6.1749717500524298E-2</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -6346,7 +6348,7 @@
         <v>0.28742937853107342</v>
       </c>
       <c r="G205">
-        <v>5.0143115661243298E-2</v>
+        <v>5.0143115661243257E-2</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -6369,7 +6371,7 @@
         <v>0.27743694614860259</v>
       </c>
       <c r="G206">
-        <v>4.5748488551713498E-2</v>
+        <v>4.5748488551713547E-2</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -6392,7 +6394,7 @@
         <v>0.36017699115044249</v>
       </c>
       <c r="G207">
-        <v>0.20582095638264841</v>
+        <v>0.20582095638264869</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -6415,7 +6417,7 @@
         <v>0.36049601417183352</v>
       </c>
       <c r="G208">
-        <v>0.33407332901780679</v>
+        <v>0.33407332901780712</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -6461,7 +6463,7 @@
         <v>0.37546125461254609</v>
       </c>
       <c r="G210">
-        <v>0.45604910175071689</v>
+        <v>0.45604910175071722</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -6484,7 +6486,7 @@
         <v>0.36732851985559573</v>
       </c>
       <c r="G211">
-        <v>0.42242364863234838</v>
+        <v>0.42242364863234821</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6507,7 +6509,7 @@
         <v>0.39784946236559138</v>
       </c>
       <c r="G212">
-        <v>0.90567576108789483</v>
+        <v>0.90567576108789472</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6530,7 +6532,7 @@
         <v>0.33035714285714279</v>
       </c>
       <c r="G213">
-        <v>0.30062731055337821</v>
+        <v>0.30062731055337799</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -6576,7 +6578,7 @@
         <v>0.36274509803921567</v>
       </c>
       <c r="G215">
-        <v>0.35707960143790313</v>
+        <v>0.35707960143790318</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6599,7 +6601,7 @@
         <v>0.34579439252336452</v>
       </c>
       <c r="G216">
-        <v>0.18155799788060659</v>
+        <v>0.1815579978806067</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
@@ -6691,7 +6693,7 @@
         <v>0.30532633158289568</v>
       </c>
       <c r="G220">
-        <v>6.5100523178898723E-2</v>
+        <v>6.510052317889875E-2</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -6714,7 +6716,7 @@
         <v>0.34816082121471342</v>
       </c>
       <c r="G221">
-        <v>0.3043793380776984</v>
+        <v>0.30437933807769801</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -6737,7 +6739,7 @@
         <v>0.33775933609958508</v>
       </c>
       <c r="G222">
-        <v>0.1814597585829705</v>
+        <v>0.1814597585829707</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -6760,7 +6762,7 @@
         <v>0.3207249802994484</v>
       </c>
       <c r="G223">
-        <v>7.3361477163654987E-2</v>
+        <v>7.3361477163655042E-2</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -6783,7 +6785,7 @@
         <v>0.36932849364791293</v>
       </c>
       <c r="G224">
-        <v>0.47785310824014587</v>
+        <v>0.4778531082401456</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -6806,7 +6808,7 @@
         <v>0.33143322475570031</v>
       </c>
       <c r="G225">
-        <v>0.13574839592918531</v>
+        <v>0.13574839592918539</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -6852,7 +6854,7 @@
         <v>0.32275971451229191</v>
       </c>
       <c r="G227">
-        <v>9.8460883379257153E-2</v>
+        <v>9.8460883379257264E-2</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -6875,7 +6877,7 @@
         <v>0.36832579185520359</v>
       </c>
       <c r="G228">
-        <v>0.32232875005644612</v>
+        <v>0.32232875005644601</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -6921,7 +6923,7 @@
         <v>0.35025817555938038</v>
       </c>
       <c r="G230">
-        <v>0.19808035640175681</v>
+        <v>0.19808035640175689</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -6944,7 +6946,7 @@
         <v>0.33775933609958508</v>
       </c>
       <c r="G231">
-        <v>0.17810352483267869</v>
+        <v>0.1781035248326788</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -6967,7 +6969,7 @@
         <v>0.32430278884462149</v>
       </c>
       <c r="G232">
-        <v>8.2010455155790599E-2</v>
+        <v>8.2010455155790543E-2</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -6990,7 +6992,7 @@
         <v>0.34845890410958902</v>
       </c>
       <c r="G233">
-        <v>0.20803815916980409</v>
+        <v>0.20803815916980431</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -7013,7 +7015,7 @@
         <v>0.26971504307488398</v>
       </c>
       <c r="G234">
-        <v>4.2014435916965881E-2</v>
+        <v>4.2014435916965943E-2</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -7082,7 +7084,7 @@
         <v>0.2172984516817939</v>
       </c>
       <c r="G237">
-        <v>2.8774998044231248E-3</v>
+        <v>2.8774998044231261E-3</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -7105,7 +7107,7 @@
         <v>0.26514657980456019</v>
       </c>
       <c r="G238">
-        <v>2.101262728767719E-2</v>
+        <v>2.1012627287677211E-2</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -7128,7 +7130,7 @@
         <v>0.28185595567867028</v>
       </c>
       <c r="G239">
-        <v>6.2898248565533291E-2</v>
+        <v>6.2898248565533221E-2</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
@@ -7151,7 +7153,7 @@
         <v>0.27315436241610741</v>
       </c>
       <c r="G240">
-        <v>2.8684689760004791E-2</v>
+        <v>2.868468976000477E-2</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -7174,7 +7176,7 @@
         <v>0.36699729486023452</v>
       </c>
       <c r="G241">
-        <v>0.23740721623564751</v>
+        <v>0.23740721623564731</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -7220,7 +7222,7 @@
         <v>0.26258064516129032</v>
       </c>
       <c r="G243">
-        <v>2.672379503140733E-2</v>
+        <v>2.672379503140734E-2</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -7243,7 +7245,7 @@
         <v>0.2600638977635783</v>
       </c>
       <c r="G244">
-        <v>1.354646547955758E-2</v>
+        <v>1.3546465479557601E-2</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -7289,7 +7291,7 @@
         <v>0.239835002946376</v>
       </c>
       <c r="G246">
-        <v>7.4969659431920804E-3</v>
+        <v>7.4969659431920873E-3</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -7312,7 +7314,7 @@
         <v>0.23404255319148939</v>
       </c>
       <c r="G247">
-        <v>4.0947088886526296E-3</v>
+        <v>4.0947088886526314E-3</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -7335,7 +7337,7 @@
         <v>0.26106478511866582</v>
       </c>
       <c r="G248">
-        <v>1.267589699580267E-2</v>
+        <v>1.2675896995802681E-2</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -7358,7 +7360,7 @@
         <v>0.25645872715815998</v>
       </c>
       <c r="G249">
-        <v>1.384503420896945E-2</v>
+        <v>1.384503420896944E-2</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -7381,7 +7383,7 @@
         <v>0.24503311258278149</v>
       </c>
       <c r="G250">
-        <v>5.1583139933614351E-3</v>
+        <v>5.1583139933614412E-3</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -7404,7 +7406,7 @@
         <v>0.25857687420584502</v>
       </c>
       <c r="G251">
-        <v>1.308523584657831E-2</v>
+        <v>1.308523584657832E-2</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -7450,7 +7452,7 @@
         <v>0.24342105263157901</v>
       </c>
       <c r="G253">
-        <v>1.871850901075512E-2</v>
+        <v>1.8718509010755131E-2</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -7473,7 +7475,7 @@
         <v>0.27668252889191031</v>
       </c>
       <c r="G254">
-        <v>4.0754784887857019E-2</v>
+        <v>4.0754784887856978E-2</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -7496,7 +7498,7 @@
         <v>0.27668252889191031</v>
       </c>
       <c r="G255">
-        <v>4.0754784887857012E-2</v>
+        <v>4.0754784887856971E-2</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -7519,7 +7521,7 @@
         <v>0.27668252889191031</v>
       </c>
       <c r="G256">
-        <v>4.0754784887857033E-2</v>
+        <v>4.0754784887857012E-2</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -7542,7 +7544,7 @@
         <v>0.31871574001566172</v>
       </c>
       <c r="G257">
-        <v>0.11209198283378791</v>
+        <v>0.112091982833788</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -7565,7 +7567,7 @@
         <v>0.31871574001566172</v>
       </c>
       <c r="G258">
-        <v>9.1498157172319863E-2</v>
+        <v>9.1498157172319947E-2</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
@@ -7588,7 +7590,7 @@
         <v>0.32327243844320891</v>
       </c>
       <c r="G259">
-        <v>0.19498296741845381</v>
+        <v>0.19498296741845361</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -7611,7 +7613,7 @@
         <v>0.30601503759398502</v>
       </c>
       <c r="G260">
-        <v>0.1347165417405409</v>
+        <v>0.13471654174054101</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -7634,7 +7636,7 @@
         <v>0.37271062271062272</v>
       </c>
       <c r="G261">
-        <v>0.60008352691046807</v>
+        <v>0.60008352691046773</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -7657,7 +7659,7 @@
         <v>0.37033666969972701</v>
       </c>
       <c r="G262">
-        <v>0.5311783038462039</v>
+        <v>0.53117830384620413</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
@@ -7703,7 +7705,7 @@
         <v>0.34608843537414968</v>
       </c>
       <c r="G264">
-        <v>0.22917860131119519</v>
+        <v>0.229178601311195</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
@@ -7726,7 +7728,7 @@
         <v>0.33973288814691149</v>
       </c>
       <c r="G265">
-        <v>0.18435798924198929</v>
+        <v>0.18435798924198901</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -7749,7 +7751,7 @@
         <v>0.33197389885807499</v>
       </c>
       <c r="G266">
-        <v>0.20437731646722379</v>
+        <v>0.20437731646722371</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -7772,7 +7774,7 @@
         <v>0.33197389885807499</v>
       </c>
       <c r="G267">
-        <v>0.2043773164672239</v>
+        <v>0.20437731646722371</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
@@ -7818,7 +7820,7 @@
         <v>0.36469534050179209</v>
       </c>
       <c r="G269">
-        <v>0.55111245241321238</v>
+        <v>0.55111245241321172</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
@@ -7841,7 +7843,7 @@
         <v>0.35890652557319219</v>
       </c>
       <c r="G270">
-        <v>0.54465408304745089</v>
+        <v>0.54465408304745011</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
@@ -7864,7 +7866,7 @@
         <v>0.31796875000000002</v>
       </c>
       <c r="G271">
-        <v>0.22396674072017439</v>
+        <v>0.22396674072017431</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
@@ -7910,7 +7912,7 @@
         <v>0.33388022969647252</v>
       </c>
       <c r="G273">
-        <v>0.25292729328137747</v>
+        <v>0.25292729328137731</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
@@ -7933,7 +7935,7 @@
         <v>0.33388022969647252</v>
       </c>
       <c r="G274">
-        <v>0.23232589425569089</v>
+        <v>0.2323258942556907</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
@@ -7956,7 +7958,7 @@
         <v>0.31574864235841738</v>
       </c>
       <c r="G275">
-        <v>0.1740767312863748</v>
+        <v>0.17407673128637469</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
@@ -8002,7 +8004,7 @@
         <v>0.32875605815831987</v>
       </c>
       <c r="G277">
-        <v>0.15420842657080541</v>
+        <v>0.1542084265708055</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
@@ -8025,7 +8027,7 @@
         <v>0.29365079365079372</v>
       </c>
       <c r="G278">
-        <v>7.1498054268873415E-2</v>
+        <v>7.1498054268873373E-2</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
@@ -8048,7 +8050,7 @@
         <v>0.29343907714491713</v>
       </c>
       <c r="G279">
-        <v>6.7786662729789476E-2</v>
+        <v>6.778666272978949E-2</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -8071,7 +8073,7 @@
         <v>0.30833333333333329</v>
       </c>
       <c r="G280">
-        <v>9.4782629036974653E-2</v>
+        <v>9.4782629036974639E-2</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -8094,7 +8096,7 @@
         <v>0.23580533024333719</v>
       </c>
       <c r="G281">
-        <v>5.9616613608623574E-3</v>
+        <v>5.96166136086236E-3</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
@@ -8140,7 +8142,7 @@
         <v>0.30786686838124061</v>
       </c>
       <c r="G283">
-        <v>9.4782629036974667E-2</v>
+        <v>9.4782629036974653E-2</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
@@ -8163,7 +8165,7 @@
         <v>0.35299219427580231</v>
       </c>
       <c r="G284">
-        <v>0.29102379643856308</v>
+        <v>0.29102379643856291</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
@@ -8186,7 +8188,7 @@
         <v>0.34845890410958902</v>
       </c>
       <c r="G285">
-        <v>0.24439751278878349</v>
+        <v>0.24439751278878369</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
@@ -8209,7 +8211,7 @@
         <v>0.26882430647291938</v>
       </c>
       <c r="G286">
-        <v>3.6176672141552971E-2</v>
+        <v>3.617667214155295E-2</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
@@ -8278,7 +8280,7 @@
         <v>0.33035714285714279</v>
       </c>
       <c r="G289">
-        <v>0.2243650854473655</v>
+        <v>0.22436508544736561</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
@@ -8301,7 +8303,7 @@
         <v>0.29471397538015931</v>
       </c>
       <c r="G290">
-        <v>8.4918206259041548E-2</v>
+        <v>8.4918206259041507E-2</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
@@ -8324,7 +8326,7 @@
         <v>0.29471397538015931</v>
       </c>
       <c r="G291">
-        <v>8.4918206259041576E-2</v>
+        <v>8.4918206259041548E-2</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
@@ -8347,7 +8349,7 @@
         <v>0.29407514450867051</v>
       </c>
       <c r="G292">
-        <v>5.8836737823406607E-2</v>
+        <v>5.8836737823406593E-2</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
@@ -8370,7 +8372,7 @@
         <v>0.27743694614860259</v>
       </c>
       <c r="G293">
-        <v>2.646202098980751E-2</v>
+        <v>2.6462020989807551E-2</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
@@ -8393,7 +8395,7 @@
         <v>0.27743694614860259</v>
       </c>
       <c r="G294">
-        <v>2.646202098980753E-2</v>
+        <v>2.6462020989807551E-2</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
@@ -8416,7 +8418,7 @@
         <v>0.34638297872340418</v>
       </c>
       <c r="G295">
-        <v>0.27393799876843072</v>
+        <v>0.27393799876843089</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
@@ -8485,7 +8487,7 @@
         <v>0.2744436952124073</v>
       </c>
       <c r="G298">
-        <v>3.0254994356047161E-2</v>
+        <v>3.0254994356047182E-2</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">
@@ -8531,7 +8533,7 @@
         <v>0.28185595567867028</v>
       </c>
       <c r="G300">
-        <v>3.470144239566969E-2</v>
+        <v>3.4701442395669718E-2</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.25">
@@ -8554,7 +8556,7 @@
         <v>0.28702397743300417</v>
       </c>
       <c r="G301">
-        <v>4.3605043334766107E-2</v>
+        <v>4.3605043334766141E-2</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
@@ -8577,7 +8579,7 @@
         <v>0.28702397743300417</v>
       </c>
       <c r="G302">
-        <v>4.3605043334766121E-2</v>
+        <v>4.3605043334766128E-2</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
@@ -8600,7 +8602,7 @@
         <v>0.28702397743300417</v>
       </c>
       <c r="G303">
-        <v>4.3605043334766128E-2</v>
+        <v>4.3605043334766141E-2</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
@@ -8669,7 +8671,7 @@
         <v>0.29948491537895511</v>
       </c>
       <c r="G306">
-        <v>5.1042088657323133E-2</v>
+        <v>5.1042088657323112E-2</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
@@ -8715,7 +8717,7 @@
         <v>0.32224861441013458</v>
       </c>
       <c r="G308">
-        <v>8.9601371462869867E-2</v>
+        <v>8.9601371462869811E-2</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
@@ -8738,7 +8740,7 @@
         <v>0.28702397743300417</v>
       </c>
       <c r="G309">
-        <v>4.5886574475827682E-2</v>
+        <v>4.5886574475827689E-2</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
@@ -8761,7 +8763,7 @@
         <v>0.28702397743300417</v>
       </c>
       <c r="G310">
-        <v>4.5886574475827703E-2</v>
+        <v>4.5886574475827689E-2</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.25">
@@ -8784,7 +8786,7 @@
         <v>0.30373134328358209</v>
       </c>
       <c r="G311">
-        <v>7.5109787386259577E-2</v>
+        <v>7.5109787386259549E-2</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
@@ -8807,7 +8809,7 @@
         <v>0.30373134328358209</v>
       </c>
       <c r="G312">
-        <v>7.5109787386259536E-2</v>
+        <v>7.5109787386259549E-2</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
@@ -8830,7 +8832,7 @@
         <v>0.27151434289526349</v>
       </c>
       <c r="G313">
-        <v>1.876438661678255E-2</v>
+        <v>1.876438661678257E-2</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
@@ -8853,7 +8855,7 @@
         <v>0.27151434289526349</v>
       </c>
       <c r="G314">
-        <v>1.876438661678256E-2</v>
+        <v>1.8764386616782581E-2</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.25">
@@ -8899,7 +8901,7 @@
         <v>0.31821735731039869</v>
       </c>
       <c r="G316">
-        <v>9.3485663622286802E-2</v>
+        <v>9.3485663622286788E-2</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.25">
@@ -8968,7 +8970,7 @@
         <v>0.21928879310344829</v>
       </c>
       <c r="G319">
-        <v>2.1267853998026358E-3</v>
+        <v>2.1267853998026402E-3</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
@@ -8991,7 +8993,7 @@
         <v>0.21928879310344829</v>
       </c>
       <c r="G320">
-        <v>2.1267853998026341E-3</v>
+        <v>2.126785399802641E-3</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.25">
@@ -9014,7 +9016,7 @@
         <v>0.21928879310344829</v>
       </c>
       <c r="G321">
-        <v>2.1267853998026328E-3</v>
+        <v>2.1267853998026419E-3</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
@@ -9037,7 +9039,7 @@
         <v>0.33251633986928097</v>
       </c>
       <c r="G322">
-        <v>0.2265591522373768</v>
+        <v>0.22655915223737669</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.25">
@@ -9060,7 +9062,7 @@
         <v>0.30237741456166423</v>
       </c>
       <c r="G323">
-        <v>8.3899787461878955E-2</v>
+        <v>8.3899787461878941E-2</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.25">
@@ -9083,7 +9085,7 @@
         <v>0.29450072358900142</v>
       </c>
       <c r="G324">
-        <v>5.0646342737648772E-2</v>
+        <v>5.0646342737648779E-2</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.25">
@@ -9106,7 +9108,7 @@
         <v>0.3039581777445855</v>
       </c>
       <c r="G325">
-        <v>7.5595640938518061E-2</v>
+        <v>7.5595640938518158E-2</v>
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.25">
@@ -9129,7 +9131,7 @@
         <v>0.21928879310344829</v>
       </c>
       <c r="G326">
-        <v>2.1267853998026358E-3</v>
+        <v>2.126785399802641E-3</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.25">
@@ -9152,7 +9154,7 @@
         <v>0.29948491537895511</v>
       </c>
       <c r="G327">
-        <v>5.1042088657323119E-2</v>
+        <v>5.1042088657323112E-2</v>
       </c>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.25">
@@ -9175,7 +9177,7 @@
         <v>0.36732851985559573</v>
       </c>
       <c r="G328">
-        <v>0.60016298264087853</v>
+        <v>0.60016298264087875</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
@@ -9198,7 +9200,7 @@
         <v>0.29970544918998532</v>
       </c>
       <c r="G329">
-        <v>8.6311975315971026E-2</v>
+        <v>8.6311975315971068E-2</v>
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.25">
@@ -9221,7 +9223,7 @@
         <v>0.28926794598436389</v>
       </c>
       <c r="G330">
-        <v>6.2873719964422106E-2</v>
+        <v>6.2873719964422134E-2</v>
       </c>
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.25">
@@ -9244,7 +9246,7 @@
         <v>0.31673151750972761</v>
       </c>
       <c r="G331">
-        <v>6.8433925934765036E-2</v>
+        <v>6.8433925934765008E-2</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.25">
@@ -9267,7 +9269,7 @@
         <v>0.34995700773860711</v>
       </c>
       <c r="G332">
-        <v>0.51811052602840957</v>
+        <v>0.5181105260284089</v>
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.25">
@@ -9336,7 +9338,7 @@
         <v>0.26793943383805141</v>
       </c>
       <c r="G335">
-        <v>3.5592886456853649E-2</v>
+        <v>3.5592886456853663E-2</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
@@ -9382,7 +9384,7 @@
         <v>0.22338090010976949</v>
       </c>
       <c r="G337">
-        <v>1.428535840187959E-2</v>
+        <v>1.428535840187958E-2</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.25">
@@ -9405,7 +9407,7 @@
         <v>0.18267504488330341</v>
       </c>
       <c r="G338">
-        <v>8.9852402360914225E-4</v>
+        <v>8.9852402360914832E-4</v>
       </c>
     </row>
     <row r="339" spans="1:7" x14ac:dyDescent="0.25">
@@ -9428,7 +9430,7 @@
         <v>0.22338090010976949</v>
       </c>
       <c r="G339">
-        <v>1.428535840187958E-2</v>
+        <v>1.428535840187959E-2</v>
       </c>
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.25">
@@ -9451,7 +9453,7 @@
         <v>0.18267504488330341</v>
       </c>
       <c r="G340">
-        <v>8.9852402360914518E-4</v>
+        <v>8.9852402360914583E-4</v>
       </c>
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.25">
@@ -9474,7 +9476,7 @@
         <v>0.27724795640326982</v>
       </c>
       <c r="G341">
-        <v>2.4357075977507109E-2</v>
+        <v>2.4357075977507098E-2</v>
       </c>
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.25">
@@ -9497,7 +9499,7 @@
         <v>0.2426952892069171</v>
       </c>
       <c r="G342">
-        <v>2.8843992373287761E-2</v>
+        <v>2.884399237328775E-2</v>
       </c>
     </row>
     <row r="343" spans="1:7" x14ac:dyDescent="0.25">
@@ -9520,7 +9522,7 @@
         <v>0.22916666666666671</v>
       </c>
       <c r="G343">
-        <v>1.457531968818644E-2</v>
+        <v>1.4575319688186429E-2</v>
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.25">
@@ -9543,7 +9545,7 @@
         <v>0.18652612282309811</v>
       </c>
       <c r="G344">
-        <v>9.1676208066965466E-4</v>
+        <v>9.167620806696552E-4</v>
       </c>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.25">
@@ -9566,7 +9568,7 @@
         <v>0.3192156862745098</v>
       </c>
       <c r="G345">
-        <v>0.1070111804932198</v>
+        <v>0.10701118049321991</v>
       </c>
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.25">
@@ -9589,7 +9591,7 @@
         <v>0.27724795640326982</v>
       </c>
       <c r="G346">
-        <v>2.4357075977507081E-2</v>
+        <v>2.4357075977507098E-2</v>
       </c>
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.25">
@@ -9635,7 +9637,7 @@
         <v>0.34845890410958902</v>
       </c>
       <c r="G348">
-        <v>0.43385984786168569</v>
+        <v>0.4338598478616853</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -9658,7 +9660,7 @@
         <v>0.30786686838124061</v>
       </c>
       <c r="G349">
-        <v>0.17253561518940491</v>
+        <v>0.1725356151894048</v>
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
@@ -9681,7 +9683,7 @@
         <v>0.2907142857142857</v>
       </c>
       <c r="G350">
-        <v>6.7395951135875071E-2</v>
+        <v>6.7395951135875098E-2</v>
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
@@ -9704,7 +9706,7 @@
         <v>0.29751461988304101</v>
       </c>
       <c r="G351">
-        <v>5.4546560751565602E-2</v>
+        <v>5.4546560751565637E-2</v>
       </c>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
@@ -9727,7 +9729,7 @@
         <v>0.22968397291196391</v>
       </c>
       <c r="G352">
-        <v>5.2848127167420579E-3</v>
+        <v>5.2848127167420692E-3</v>
       </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
@@ -9750,7 +9752,7 @@
         <v>0.18686868686868691</v>
       </c>
       <c r="G353">
-        <v>3.3240546387992538E-4</v>
+        <v>3.3240546387992891E-4</v>
       </c>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
@@ -9773,7 +9775,7 @@
         <v>0.2367655613728912</v>
       </c>
       <c r="G354">
-        <v>1.318664577369022E-2</v>
+        <v>1.3186645773690209E-2</v>
       </c>
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
@@ -9796,7 +9798,7 @@
         <v>0.19152941176470589</v>
       </c>
       <c r="G355">
-        <v>8.2941692361920046E-4</v>
+        <v>8.2941692361920122E-4</v>
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
@@ -9819,7 +9821,7 @@
         <v>0.2367655613728912</v>
       </c>
       <c r="G356">
-        <v>1.318664577369022E-2</v>
+        <v>1.3186645773690209E-2</v>
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
@@ -9842,7 +9844,7 @@
         <v>0.19152941176470589</v>
       </c>
       <c r="G357">
-        <v>8.2941692361919862E-4</v>
+        <v>8.294169236192009E-4</v>
       </c>
     </row>
     <row r="358" spans="1:7" x14ac:dyDescent="0.25">
@@ -9865,7 +9867,7 @@
         <v>0.22955442752397071</v>
       </c>
       <c r="G358">
-        <v>1.149236003974422E-2</v>
+        <v>1.149236003974421E-2</v>
       </c>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.25">
@@ -9888,7 +9890,7 @@
         <v>0.1867829279486003</v>
       </c>
       <c r="G359">
-        <v>7.2284931838442702E-4</v>
+        <v>7.2284931838442962E-4</v>
       </c>
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.25">
@@ -9911,7 +9913,7 @@
         <v>0.22955442752397071</v>
       </c>
       <c r="G360">
-        <v>1.1492360039744231E-2</v>
+        <v>1.149236003974422E-2</v>
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
@@ -9934,7 +9936,7 @@
         <v>0.1867829279486003</v>
       </c>
       <c r="G361">
-        <v>7.2284931838442474E-4</v>
+        <v>7.2284931838442919E-4</v>
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
@@ -9957,7 +9959,7 @@
         <v>0.35025817555938038</v>
       </c>
       <c r="G362">
-        <v>0.42847210713913392</v>
+        <v>0.42847210713913381</v>
       </c>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
@@ -9980,7 +9982,7 @@
         <v>0.19960765080922019</v>
       </c>
       <c r="G363">
-        <v>3.5662758647151162E-3</v>
+        <v>3.566275864715117E-3</v>
       </c>
     </row>
     <row r="364" spans="1:7" x14ac:dyDescent="0.25">
@@ -10003,7 +10005,7 @@
         <v>0.29238505747126442</v>
       </c>
       <c r="G364">
-        <v>3.1387643685038429E-2</v>
+        <v>3.1387643685038408E-2</v>
       </c>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
@@ -10026,7 +10028,7 @@
         <v>0.21928879310344829</v>
       </c>
       <c r="G365">
-        <v>2.1267853998026371E-3</v>
+        <v>2.126785399802638E-3</v>
       </c>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.25">
@@ -10049,7 +10051,7 @@
         <v>0.3197172034564022</v>
       </c>
       <c r="G366">
-        <v>9.1337305871967228E-2</v>
+        <v>9.1337305871967145E-2</v>
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
@@ -10072,7 +10074,7 @@
         <v>0.25358255451713402</v>
       </c>
       <c r="G367">
-        <v>1.9659303746696589E-2</v>
+        <v>1.96593037466966E-2</v>
       </c>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
@@ -10095,7 +10097,7 @@
         <v>0.28783592644978778</v>
       </c>
       <c r="G368">
-        <v>4.3143706718413888E-2</v>
+        <v>4.3143706718413881E-2</v>
       </c>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.25">
@@ -10164,7 +10166,7 @@
         <v>0.28783592644978778</v>
       </c>
       <c r="G371">
-        <v>4.3143706718413881E-2</v>
+        <v>4.3143706718413867E-2</v>
       </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
@@ -10187,7 +10189,7 @@
         <v>0.29970544918998532</v>
       </c>
       <c r="G372">
-        <v>5.3168553280372143E-2</v>
+        <v>5.3168553280372191E-2</v>
       </c>
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.25">
@@ -10256,7 +10258,7 @@
         <v>0.32173913043478258</v>
       </c>
       <c r="G375">
-        <v>9.4388560873654118E-2</v>
+        <v>9.4388560873654104E-2</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
@@ -10279,7 +10281,7 @@
         <v>0.31896551724137928</v>
       </c>
       <c r="G376">
-        <v>6.841837362632712E-2</v>
+        <v>6.8418373626327134E-2</v>
       </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
@@ -10302,7 +10304,7 @@
         <v>0.23204104903078679</v>
       </c>
       <c r="G377">
-        <v>1.380397331575605E-2</v>
+        <v>1.3803973315756061E-2</v>
       </c>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.25">
@@ -10325,7 +10327,7 @@
         <v>0.2277560156687185</v>
       </c>
       <c r="G378">
-        <v>8.2371150464672447E-3</v>
+        <v>8.2371150464672412E-3</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
@@ -10348,7 +10350,7 @@
         <v>0.22801120448179271</v>
       </c>
       <c r="G379">
-        <v>8.237115046467236E-3</v>
+        <v>8.2371150464672447E-3</v>
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
@@ -10371,7 +10373,7 @@
         <v>0.1857599269739845</v>
       </c>
       <c r="G380">
-        <v>5.1810010965558622E-4</v>
+        <v>5.1810010965558709E-4</v>
       </c>
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.25">
@@ -10394,7 +10396,7 @@
         <v>0.3371996685998343</v>
       </c>
       <c r="G381">
-        <v>0.29682948250275709</v>
+        <v>0.29682948250275698</v>
       </c>
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.25">
@@ -10417,7 +10419,7 @@
         <v>0.35177182368193599</v>
       </c>
       <c r="G382">
-        <v>0.313506265754049</v>
+        <v>0.31350626575404911</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
@@ -10440,7 +10442,7 @@
         <v>0.32123125493291238</v>
       </c>
       <c r="G383">
-        <v>9.9762852093368382E-2</v>
+        <v>9.9762852093368423E-2</v>
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
@@ -10463,7 +10465,7 @@
         <v>0.30305286671630682</v>
       </c>
       <c r="G384">
-        <v>5.7348500091208267E-2</v>
+        <v>5.7348500091208239E-2</v>
       </c>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.25">
@@ -10486,7 +10488,7 @@
         <v>0.2755585646580907</v>
       </c>
       <c r="G385">
-        <v>1.9578046424815469E-2</v>
+        <v>1.957804642481548E-2</v>
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.25">
@@ -10509,7 +10511,7 @@
         <v>0.30647590361445781</v>
       </c>
       <c r="G386">
-        <v>0.1223306067373804</v>
+        <v>0.1223306067373805</v>
       </c>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.25">
@@ -10532,7 +10534,7 @@
         <v>0.3039581777445855</v>
       </c>
       <c r="G387">
-        <v>4.893726282587374E-2</v>
+        <v>4.8937262825873747E-2</v>
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.25">
@@ -10555,7 +10557,7 @@
         <v>0.23007348784624079</v>
       </c>
       <c r="G388">
-        <v>8.2630744580017659E-4</v>
+        <v>8.2630744580018364E-4</v>
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.25">
@@ -10578,7 +10580,7 @@
         <v>0.2868217054263566</v>
       </c>
       <c r="G389">
-        <v>4.0900908925180238E-2</v>
+        <v>4.0900908925180217E-2</v>
       </c>
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.25">
@@ -10601,7 +10603,7 @@
         <v>0.23204104903078679</v>
       </c>
       <c r="G390">
-        <v>1.380397331575605E-2</v>
+        <v>1.3803973315756061E-2</v>
       </c>
     </row>
     <row r="391" spans="1:7" x14ac:dyDescent="0.25">
@@ -10624,7 +10626,7 @@
         <v>0.27061170212765961</v>
       </c>
       <c r="G391">
-        <v>3.6360601364131558E-2</v>
+        <v>3.6360601364131537E-2</v>
       </c>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.25">
@@ -10647,7 +10649,7 @@
         <v>0.21253263707571801</v>
       </c>
       <c r="G392">
-        <v>2.6426344336459881E-3</v>
+        <v>2.642634433645992E-3</v>
       </c>
     </row>
     <row r="393" spans="1:7" x14ac:dyDescent="0.25">
@@ -10670,7 +10672,7 @@
         <v>0.21253263707571801</v>
       </c>
       <c r="G393">
-        <v>2.6426344336459881E-3</v>
+        <v>2.642634433645992E-3</v>
       </c>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.25">
@@ -10693,7 +10695,7 @@
         <v>0.24711596842744379</v>
       </c>
       <c r="G394">
-        <v>2.2118370035802418E-2</v>
+        <v>2.2118370035802411E-2</v>
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.25">
@@ -10716,7 +10718,7 @@
         <v>0.32769726247987119</v>
       </c>
       <c r="G395">
-        <v>0.17806626632978009</v>
+        <v>0.17806626632978001</v>
       </c>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.25">
@@ -10739,7 +10741,7 @@
         <v>0.26882430647291938</v>
       </c>
       <c r="G396">
-        <v>3.7873387187865398E-2</v>
+        <v>3.7873387187865322E-2</v>
       </c>
     </row>
     <row r="397" spans="1:7" x14ac:dyDescent="0.25">
@@ -10762,7 +10764,7 @@
         <v>0.23539618276460381</v>
       </c>
       <c r="G397">
-        <v>7.8630759040955386E-3</v>
+        <v>7.8630759040955438E-3</v>
       </c>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.25">
@@ -10785,7 +10787,7 @@
         <v>0.23539618276460381</v>
       </c>
       <c r="G398">
-        <v>7.8630759040955352E-3</v>
+        <v>7.8630759040955386E-3</v>
       </c>
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.25">
@@ -10808,7 +10810,7 @@
         <v>0.2172984516817939</v>
       </c>
       <c r="G399">
-        <v>2.8774998044231248E-3</v>
+        <v>2.87749980442313E-3</v>
       </c>
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.25">
@@ -10831,7 +10833,7 @@
         <v>0.24298507462686569</v>
       </c>
       <c r="G400">
-        <v>4.6143084257742571E-3</v>
+        <v>4.6143084257742693E-3</v>
       </c>
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.25">
@@ -10854,7 +10856,7 @@
         <v>0.3123561013046815</v>
       </c>
       <c r="G401">
-        <v>0.12571407743035579</v>
+        <v>0.12571407743035559</v>
       </c>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
@@ -10900,7 +10902,7 @@
         <v>0.24415116976604681</v>
       </c>
       <c r="G403">
-        <v>6.1930171167704929E-3</v>
+        <v>6.1930171167704972E-3</v>
       </c>
     </row>
     <row r="404" spans="1:7" x14ac:dyDescent="0.25">
@@ -10923,7 +10925,7 @@
         <v>0.27315436241610741</v>
       </c>
       <c r="G404">
-        <v>2.8684689760004801E-2</v>
+        <v>2.868468976000477E-2</v>
       </c>
     </row>
     <row r="405" spans="1:7" x14ac:dyDescent="0.25">
@@ -10946,7 +10948,7 @@
         <v>0.29948491537895511</v>
       </c>
       <c r="G405">
-        <v>4.7097292867898821E-2</v>
+        <v>4.709729286789878E-2</v>
       </c>
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.25">
@@ -10992,7 +10994,7 @@
         <v>0.28205128205128199</v>
       </c>
       <c r="G407">
-        <v>2.1362016267315209E-2</v>
+        <v>2.136201626731523E-2</v>
       </c>
     </row>
     <row r="408" spans="1:7" x14ac:dyDescent="0.25">
@@ -11015,7 +11017,7 @@
         <v>0.23404255319148939</v>
       </c>
       <c r="G408">
-        <v>4.0947088886526288E-3</v>
+        <v>4.0947088886526314E-3</v>
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.25">
@@ -11038,7 +11040,7 @@
         <v>0.28224687933425802</v>
       </c>
       <c r="G409">
-        <v>2.9087263452183761E-2</v>
+        <v>2.9087263452183799E-2</v>
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.25">
@@ -11061,7 +11063,7 @@
         <v>0.28146611341632088</v>
       </c>
       <c r="G410">
-        <v>2.1144735962883712E-2</v>
+        <v>2.1144735962883719E-2</v>
       </c>
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.25">
@@ -11084,7 +11086,7 @@
         <v>0.24503311258278149</v>
       </c>
       <c r="G411">
-        <v>5.1583139933614342E-3</v>
+        <v>5.1583139933614377E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>